<commit_message>
Update DateBase/orders/Fresh bloom Flowers_2025-11-23.xlsx
</commit_message>
<xml_diff>
--- a/DateBase/orders/Fresh bloom Flowers_2025-11-23.xlsx
+++ b/DateBase/orders/Fresh bloom Flowers_2025-11-23.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:L61"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -606,10 +606,347 @@
       <c r="C21" t="str">
         <v>579_腊梅红_wax red_undefined_1bunch</v>
       </c>
+      <c r="F21" t="str">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="C22" t="str">
+        <v>577_腊梅白_wax white_undefined_1bunch</v>
+      </c>
+      <c r="F22" t="str">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="C23" t="str">
+        <v>449_柔丽思 绿_undefined_undefined_1bunch</v>
+      </c>
+      <c r="F23" t="str">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" xml:space="preserve">
+      <c r="C24" t="str" xml:space="preserve">
+        <v xml:space="preserve">510_翠珠白_Didiscus caeruleus 
+white_Trachymene Coerulea_1bunch</v>
+      </c>
+      <c r="F24" t="str">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" xml:space="preserve">
+      <c r="A25" t="str">
+        <v>3</v>
+      </c>
+      <c r="C25" t="str" xml:space="preserve">
+        <v xml:space="preserve">345_天竺少女_Cryptomeria
+Kashiwaba_undefined_1bunch</v>
+      </c>
+      <c r="F25" t="str">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="C26" t="str">
+        <v>462_五针松_undefined_undefined_1bunch</v>
+      </c>
+      <c r="F26" t="str">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>4</v>
+      </c>
+      <c r="C27" t="str">
+        <v>597_尤加利叶小叶_undefined_undefined_1bunch</v>
+      </c>
+      <c r="F27" t="str">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="C28" t="str">
+        <v>315_尤加利叶圆叶_Eucalyptus Populus_undefined_1bunch</v>
+      </c>
+      <c r="F28" t="str">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="C29" t="str">
+        <v>462_五针松_undefined_undefined_1bunch</v>
+      </c>
+      <c r="F29" t="str">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="C30" t="str">
+        <v>431_小米果_undefined_undefined_1bunch</v>
+      </c>
+      <c r="F30" t="str">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="C31" t="str">
+        <v>221_朱丽叶塔_Julieta_Rosa rugosa Thunb._10stems</v>
+      </c>
+      <c r="F31" t="str">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="C32" t="str">
+        <v>646_芍药莎拉_Sarah_undefined_5stems</v>
+      </c>
+      <c r="F32" t="str">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="C33" t="str">
+        <v>203_佛罗伊德_Floyd_Rosa rugosa Thunb._20stems</v>
+      </c>
+      <c r="F33" t="str">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="C34" t="str">
+        <v>157_流沙_Quicksand_Rosa rugosa Thunb._20stems</v>
+      </c>
+      <c r="F34" t="str">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="C35" t="str">
+        <v>612_康乃馨古巴爱情_cuba love_undefined_20stems</v>
+      </c>
+      <c r="F35" t="str">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="C36" t="str">
+        <v>506_紫罗兰香槟色_violet champagne_undefined_1bunch</v>
+      </c>
+      <c r="F36" t="str">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="C37" t="str">
+        <v>3_波浪白洋桔梗_Wavy White Lisianthus_Eustoma grandiflorum (Raf.) Shinners_800/600g</v>
+      </c>
+      <c r="F37" t="str">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="C38" t="str">
+        <v>7_翠绿洋桔梗_Dark Green Lisianthus_Eustoma grandiflorum (Raf.) Shinners_800/600g</v>
+      </c>
+      <c r="F38" t="str">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>5</v>
+      </c>
+      <c r="C39" t="str">
+        <v>184_微光_shimmer_Rosa rugosa Thunb._20stems</v>
+      </c>
+      <c r="F39" t="str">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="C40" t="str">
+        <v>152_白荔枝_White Ohara_Rosa rugosa Thunb._20stems</v>
+      </c>
+      <c r="F40" t="str">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="C41" t="str">
+        <v>135_甜蜜曼塔_sweet menta_Rosa rugosa Thunb._20stems</v>
+      </c>
+      <c r="F41" t="str">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="C42" t="str">
+        <v>147_娜欧米_Red Naomi_Rosa rugosa Thunb._20stems</v>
+      </c>
+      <c r="F42" t="str">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="C43" t="str">
+        <v>160_卡布奇诺_Cappuccino_Rosa rugosa Thunb._20stems</v>
+      </c>
+      <c r="F43" t="str">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="C44" t="str">
+        <v>137_凯瑟琳_Catherine_Rosa rugosa Thunb._20stems</v>
+      </c>
+      <c r="F44" t="str">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="C45" t="str">
+        <v>604_康乃馨粉佳人_pink_undefined_20stems</v>
+      </c>
+      <c r="F45" t="str">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="C46" t="str">
+        <v>600_康乃馨复古红_vintage red_undefined_20stems</v>
+      </c>
+      <c r="F46" t="str">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>6</v>
+      </c>
+      <c r="C47" t="str">
+        <v>452_粉吊鸟_pink hanging heliconia_undefined_1bunch</v>
+      </c>
+      <c r="F47" t="str">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="C48" t="str">
+        <v>744_永生吊米深红_undefined_undefined_1bunch</v>
+      </c>
+      <c r="F48" t="str">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="C49" t="str">
+        <v>592_进口春兰叶_undefined_undefined_1bunch</v>
+      </c>
+      <c r="F49" t="str">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="C50" t="str">
+        <v>734_乒乓菊红_undefined_undefined_1bunch</v>
+      </c>
+      <c r="F50" t="str">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="C51" t="str">
+        <v>419_松虫草红_scabiosa watermelon_undefined_1bunch</v>
+      </c>
+      <c r="F51" t="str">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="C52" t="str">
+        <v>653_大丽花 黑_undefined_undefined_5stems</v>
+      </c>
+      <c r="F52" t="str">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="C53" t="str">
+        <v>648_洋牡丹河内_undefined_undefined_1bunch</v>
+      </c>
+      <c r="F53" t="str">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="C54" t="str">
+        <v>75_爱心_undefined_Gerbera L._10stems</v>
+      </c>
+      <c r="F54" t="str">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="C55" t="str">
+        <v>47_拉丝玫红_Spider Dark Pink_Gerbera L._20stems</v>
+      </c>
+      <c r="F55" t="str">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="str">
+        <v>7</v>
+      </c>
+      <c r="C56" t="str">
+        <v>147_娜欧米_Red Naomi_Rosa rugosa Thunb._20stems</v>
+      </c>
+      <c r="F56" t="str">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="C57" t="str">
+        <v>155_曼塔_Menta_Rosa rugosa Thunb._20stems</v>
+      </c>
+      <c r="F57" t="str">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="C58" t="str">
+        <v>192_粉荔枝_Pink Ohara_Rosa rugosa Thunb._20stems</v>
+      </c>
+      <c r="F58" t="str">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="C59" t="str">
+        <v>197_粉红雪山_Sweet Avalanche_Rosa rugosa Thunb._20stems</v>
+      </c>
+      <c r="F59" t="str">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="C60" t="str">
+        <v>144_高原红_High Plateau Red_Rosa rugosa Thunb._20stems</v>
+      </c>
+      <c r="F60" t="str">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="C61" t="str">
+        <v>794_小菊罗西香槟_undefined_undefined_1bunch</v>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L21"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L61"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -667,7 +1004,7 @@
         <v>0.00</v>
       </c>
       <c r="G2" t="str">
-        <v>05301055555555101010104010520</v>
+        <v>05301055555555101010104010525510530305510558655653111253.55555105105555652.5510650</v>
       </c>
     </row>
   </sheetData>

</xml_diff>